<commit_message>
testing booking.com search feature
</commit_message>
<xml_diff>
--- a/com.booking/src/test/resources/test_data.xlsx
+++ b/com.booking/src/test/resources/test_data.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zainj\IdeaProjects\SeleniumBootcampWinterWeekend2022\com.espn\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zainj\IdeaProjects\SeleniumBootcampWinterWeekend2022\com.booking\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7DA89EF-1238-4A00-940D-3C2E7F60B1EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E138E1DB-5904-4F12-BC0E-2E45329C7E43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{723F212A-670C-4A3B-B8E6-389E6F040CFB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Locations" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,6 +32,20 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>Locations</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>California</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -65,8 +79,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -381,14 +396,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DADF1CD2-1FEB-4105-B7FC-B561B248CD13}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="16384" width="8.7265625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>